<commit_message>
advances in obtaining data from plants / basins, improve
</commit_message>
<xml_diff>
--- a/data/reportes_por_planta.xlsx
+++ b/data/reportes_por_planta.xlsx
@@ -8,17 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Year Daily" sheetId="1" r:id="rId1"/>
-    <sheet name="El Alto" sheetId="2" r:id="rId2"/>
-    <sheet name="Tilata" sheetId="3" r:id="rId3"/>
-    <sheet name="Linea Oeste" sheetId="4" r:id="rId4"/>
-    <sheet name="San Felipe" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="253">
   <si>
     <t>Year Daily Overview</t>
   </si>
@@ -777,18 +773,6 @@
   </si>
   <si>
     <t>pHSalida</t>
-  </si>
-  <si>
-    <t>Year Daily - El Alto</t>
-  </si>
-  <si>
-    <t>Year Daily - Tilata</t>
-  </si>
-  <si>
-    <t>Year Daily - Linea Oeste</t>
-  </si>
-  <si>
-    <t>Year Daily - San Felipe</t>
   </si>
 </sst>
 </file>
@@ -972,374 +956,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Year Daily - El Alto</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'El Alto'!$A$3:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Date</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45717</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'El Alto'!$B$3:$B$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1319.851233312598</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="50020001"/>
-        <c:axId val="50020002"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50020001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50020002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50020002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50020001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Year Daily - Tilata</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tilata!$A$3:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Date</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45717</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tilata!$B$3:$B$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4666666666666667</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="50030001"/>
-        <c:axId val="50030002"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50030001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50030002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50030002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50030001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Year Daily - Linea Oeste</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Linea Oeste'!$A$3:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Date</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45717</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Linea Oeste'!$B$3:$B$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="50040001"/>
-        <c:axId val="50040002"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50040001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50040002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50040002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50040001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Year Daily - San Felipe</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'San Felipe'!$A$3:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Date</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45717</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'San Felipe'!$B$3:$B$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>261.3778230772805</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="50050001"/>
-        <c:axId val="50050002"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50050001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50050002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50050002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50050001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1352,146 +968,6 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
@@ -2841,7 +2317,7 @@
         <v>3.114748730099019</v>
       </c>
       <c r="F4" s="2">
-        <v>4.740126056050171</v>
+        <v>4.74012605605017</v>
       </c>
       <c r="G4" s="2">
         <v>4.746729369266357</v>
@@ -2892,7 +2368,7 @@
         <v>567.0523827582781</v>
       </c>
       <c r="W4" s="2">
-        <v>116.9343924399076</v>
+        <v>116.9343924399077</v>
       </c>
       <c r="X4" s="2">
         <v>17.55304392071243</v>
@@ -2967,7 +2443,7 @@
         <v>93.67562360073084</v>
       </c>
       <c r="AV4" s="2">
-        <v>306.959103373607</v>
+        <v>306.9591033736069</v>
       </c>
       <c r="AW4" s="2">
         <v>760.3767686809638</v>
@@ -3237,7 +2713,7 @@
         <v>104.2177734800965</v>
       </c>
       <c r="EH4" s="2">
-        <v>196.6018380263553</v>
+        <v>196.6018380263552</v>
       </c>
       <c r="EI4" s="2">
         <v>3.886327260525569</v>
@@ -3390,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="GK4" s="2">
-        <v>4.891052195060899</v>
+        <v>4.891052195060898</v>
       </c>
       <c r="GL4" s="2">
         <v>3.910717817276543</v>
@@ -3405,13 +2881,13 @@
         <v>2.464304743669789</v>
       </c>
       <c r="GP4" s="2">
-        <v>9.815512676436951</v>
+        <v>9.815512676436953</v>
       </c>
       <c r="GQ4" s="2">
         <v>2.324013646399337</v>
       </c>
       <c r="GR4" s="2">
-        <v>3.027998112399133</v>
+        <v>3.027998112399132</v>
       </c>
       <c r="GS4" s="2">
         <v>9.082050351582852</v>
@@ -3456,10 +2932,10 @@
         <v>1.121876632420707</v>
       </c>
       <c r="HH4" s="2">
-        <v>71.83282195777153</v>
+        <v>71.83282195777154</v>
       </c>
       <c r="HI4" s="2">
-        <v>83.36532559743958</v>
+        <v>83.36532559743955</v>
       </c>
       <c r="HJ4" s="2">
         <v>-1.212522506713867</v>
@@ -3504,7 +2980,7 @@
         <v>0.3821428571428571</v>
       </c>
       <c r="HX4" s="2">
-        <v>0.375</v>
+        <v>0.3749999999999999</v>
       </c>
       <c r="HY4" s="2">
         <v>0.3791666666666667</v>
@@ -3549,7 +3025,7 @@
         <v>4.756905955640744</v>
       </c>
       <c r="IM4" s="2">
-        <v>0.2154098974739541</v>
+        <v>0.2154098974739542</v>
       </c>
       <c r="IN4" s="2">
         <v>2.176184326284647</v>
@@ -3572,46 +3048,46 @@
         <v>45748</v>
       </c>
       <c r="B5" s="2">
-        <v>1.730564993837924</v>
+        <v>1.748150528199293</v>
       </c>
       <c r="C5" s="2">
-        <v>3.545595136367651</v>
+        <v>3.521648610857859</v>
       </c>
       <c r="D5" s="2">
-        <v>2.032666384244505</v>
+        <v>2.033443846656901</v>
       </c>
       <c r="E5" s="2">
-        <v>2.865971785579082</v>
+        <v>2.870222697067011</v>
       </c>
       <c r="F5" s="2">
-        <v>4.449964103352919</v>
+        <v>4.449136465566421</v>
       </c>
       <c r="G5" s="2">
-        <v>4.457904671110075</v>
+        <v>4.457162018490582</v>
       </c>
       <c r="H5" s="2">
-        <v>1.485742887162096</v>
+        <v>1.485806144369456</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
       </c>
       <c r="J5" s="2">
-        <v>0.5069999740212506</v>
+        <v>0.5092620790450507</v>
       </c>
       <c r="K5" s="2">
-        <v>261.0727626334767</v>
+        <v>259.5455647594307</v>
       </c>
       <c r="L5" s="2">
         <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>3.156167196938449</v>
+        <v>3.178658565878746</v>
       </c>
       <c r="N5" s="2">
-        <v>-198.1589525853312</v>
+        <v>-201.0152584044476</v>
       </c>
       <c r="O5" s="2">
-        <v>2.284022148769838</v>
+        <v>2.296590770193621</v>
       </c>
       <c r="P5" s="2">
         <v>0</v>
@@ -3620,58 +3096,58 @@
         <v>0</v>
       </c>
       <c r="R5" s="2">
-        <v>815.1032845351876</v>
+        <v>817.4673980470678</v>
       </c>
       <c r="S5" s="2">
-        <v>192.7964141944631</v>
+        <v>193.3573650827728</v>
       </c>
       <c r="T5" s="2">
         <v>0</v>
       </c>
       <c r="U5" s="2">
-        <v>1489.43851149402</v>
+        <v>1490.738055795346</v>
       </c>
       <c r="V5" s="2">
-        <v>560.0753708119049</v>
+        <v>559.4469444850155</v>
       </c>
       <c r="W5" s="2">
-        <v>152.5864834831679</v>
+        <v>153.6013034078852</v>
       </c>
       <c r="X5" s="2">
-        <v>15.92467962649384</v>
+        <v>15.66279185599618</v>
       </c>
       <c r="Y5" s="2">
-        <v>9.467649628008381</v>
+        <v>9.540952714676742</v>
       </c>
       <c r="Z5" s="2">
         <v>0</v>
       </c>
       <c r="AA5" s="2">
-        <v>17.30963873832287</v>
+        <v>17.41318588611078</v>
       </c>
       <c r="AB5" s="2">
-        <v>118.4971004143347</v>
+        <v>118.4980800872902</v>
       </c>
       <c r="AC5" s="2">
-        <v>13.47331276958803</v>
+        <v>13.17577846463515</v>
       </c>
       <c r="AD5" s="2">
-        <v>29.64665766847174</v>
+        <v>29.15044925448731</v>
       </c>
       <c r="AE5" s="2">
         <v>0</v>
       </c>
       <c r="AF5" s="2">
-        <v>8.260716818750534</v>
+        <v>8.191901625794909</v>
       </c>
       <c r="AG5" s="2">
-        <v>571.7260485071038</v>
+        <v>569.366626100429</v>
       </c>
       <c r="AH5" s="2">
-        <v>1319.058619099679</v>
+        <v>1320.450910761095</v>
       </c>
       <c r="AI5" s="2">
-        <v>0.4934327886455545</v>
+        <v>0.4912195947254377</v>
       </c>
       <c r="AJ5" s="2">
         <v>0</v>
@@ -3692,28 +3168,28 @@
         <v>0</v>
       </c>
       <c r="AP5" s="2">
-        <v>1.122214382815748</v>
+        <v>1.120985406983316</v>
       </c>
       <c r="AQ5" s="2">
-        <v>1.100243169072247</v>
+        <v>1.103470641497048</v>
       </c>
       <c r="AR5" s="2">
-        <v>59.62273103035433</v>
+        <v>59.65601994339971</v>
       </c>
       <c r="AS5" s="2">
-        <v>132.2634899600185</v>
+        <v>134.0449898859166</v>
       </c>
       <c r="AT5" s="2">
         <v>-7.5</v>
       </c>
       <c r="AU5" s="2">
-        <v>93.08555835257766</v>
+        <v>93.08290994122954</v>
       </c>
       <c r="AV5" s="2">
-        <v>315.0055251538689</v>
+        <v>315.0560057360712</v>
       </c>
       <c r="AW5" s="2">
-        <v>766.5722035504696</v>
+        <v>767.7250213931696</v>
       </c>
       <c r="AX5" s="2">
         <v>0</v>
@@ -3953,64 +3429,64 @@
         <v>0</v>
       </c>
       <c r="DY5" s="2">
-        <v>1320.925141304659</v>
+        <v>1321.092147311947</v>
       </c>
       <c r="DZ5" s="2">
-        <v>1288.979545232913</v>
+        <v>1289.354882613616</v>
       </c>
       <c r="EA5" s="2">
-        <v>587.5698348660505</v>
+        <v>587.0944930761304</v>
       </c>
       <c r="EB5" s="2">
-        <v>38.175279731724</v>
+        <v>36.70615282798361</v>
       </c>
       <c r="EC5" s="2">
-        <v>129.2812237122106</v>
+        <v>129.1333272391257</v>
       </c>
       <c r="ED5" s="2">
-        <v>588.0030654638125</v>
+        <v>586.9903816202606</v>
       </c>
       <c r="EE5" s="2">
-        <v>2449.235808673294</v>
+        <v>2448.662230153523</v>
       </c>
       <c r="EF5" s="2">
-        <v>0.5984480293666495</v>
+        <v>0.6177804719202059</v>
       </c>
       <c r="EG5" s="2">
-        <v>100.5100164461985</v>
+        <v>100.4318721156764</v>
       </c>
       <c r="EH5" s="2">
-        <v>204.4591111008556</v>
+        <v>204.5465557383561</v>
       </c>
       <c r="EI5" s="2">
-        <v>4.049516904225479</v>
+        <v>4.05469319621367</v>
       </c>
       <c r="EJ5" s="2">
-        <v>4.04512417111714</v>
+        <v>4.051644768650671</v>
       </c>
       <c r="EK5" s="2">
-        <v>8.861787353458858</v>
+        <v>8.875204885117309</v>
       </c>
       <c r="EL5" s="2">
-        <v>9.753907947205761</v>
+        <v>9.737785872571026</v>
       </c>
       <c r="EM5" s="2">
-        <v>1.102320777936239</v>
+        <v>1.095520079033786</v>
       </c>
       <c r="EN5" s="2">
-        <v>0.9313120685932672</v>
+        <v>0.9198421363004621</v>
       </c>
       <c r="EO5" s="2">
-        <v>7.565927862689803</v>
+        <v>7.562415947618795</v>
       </c>
       <c r="EP5" s="2">
-        <v>9.163425479334171</v>
+        <v>9.162425610312958</v>
       </c>
       <c r="EQ5" s="2">
-        <v>102.0020736957745</v>
+        <v>101.9273613681509</v>
       </c>
       <c r="ER5" s="2">
-        <v>2.931918662971499</v>
+        <v>2.934663036931359</v>
       </c>
       <c r="ES5" s="2">
         <v>0</v>
@@ -4025,16 +3501,16 @@
         <v>0</v>
       </c>
       <c r="EW5" s="2">
-        <v>0.5069999740212506</v>
+        <v>0.5092620790450507</v>
       </c>
       <c r="EX5" s="2">
-        <v>22.682263670369</v>
+        <v>22.86346742405141</v>
       </c>
       <c r="EY5" s="2">
-        <v>30.24610785649983</v>
+        <v>30.36360272246096</v>
       </c>
       <c r="EZ5" s="2">
-        <v>17.46304926959731</v>
+        <v>17.54461320490141</v>
       </c>
       <c r="FA5" s="2">
         <v>0</v>
@@ -4043,13 +3519,13 @@
         <v>0</v>
       </c>
       <c r="FC5" s="2">
-        <v>27.85501521740856</v>
+        <v>27.77768969560363</v>
       </c>
       <c r="FD5" s="2">
         <v>-0.1148122102022171</v>
       </c>
       <c r="FE5" s="2">
-        <v>21.90102650791603</v>
+        <v>22.0368890862813</v>
       </c>
       <c r="FF5" s="2">
         <v>0</v>
@@ -4079,115 +3555,115 @@
         <v>0</v>
       </c>
       <c r="FO5" s="2">
-        <v>128.3147064545943</v>
+        <v>127.395282821263</v>
       </c>
       <c r="FP5" s="2">
-        <v>0.2731443782847562</v>
+        <v>0.2774523797578891</v>
       </c>
       <c r="FQ5" s="2">
-        <v>4.196205452439245</v>
+        <v>4.200158573121145</v>
       </c>
       <c r="FR5" s="2">
         <v>0</v>
       </c>
       <c r="FS5" s="2">
-        <v>1.921831685227078</v>
+        <v>1.923724791038735</v>
       </c>
       <c r="FT5" s="2">
-        <v>1.931656773687066</v>
+        <v>1.933560829731381</v>
       </c>
       <c r="FU5" s="2">
-        <v>3.194813296089862</v>
+        <v>3.198298552495443</v>
       </c>
       <c r="FV5" s="2">
-        <v>5.634898422299972</v>
+        <v>5.645393620969008</v>
       </c>
       <c r="FW5" s="2">
-        <v>5.640358849545512</v>
+        <v>5.651000239047097</v>
       </c>
       <c r="FX5" s="2">
-        <v>0.19741577501168</v>
+        <v>0.1975841786766656</v>
       </c>
       <c r="FY5" s="2">
-        <v>0.05361570464166205</v>
+        <v>0.05177096410989571</v>
       </c>
       <c r="FZ5" s="2">
-        <v>2.348438040226955</v>
+        <v>2.348396894059107</v>
       </c>
       <c r="GA5" s="2">
-        <v>2.758685708638643</v>
+        <v>2.762136923608429</v>
       </c>
       <c r="GB5" s="2">
-        <v>4.471288776632328</v>
+        <v>4.472683085868825</v>
       </c>
       <c r="GC5" s="2">
         <v>-1.125</v>
       </c>
       <c r="GD5" s="2">
-        <v>3.268990440573463</v>
+        <v>3.277211544010139</v>
       </c>
       <c r="GE5" s="2">
-        <v>4.086802426777915</v>
+        <v>4.091176308989563</v>
       </c>
       <c r="GF5" s="2">
-        <v>91.47042297020555</v>
+        <v>91.47343902973857</v>
       </c>
       <c r="GG5" s="2">
-        <v>91.75473927010897</v>
+        <v>91.78248249796664</v>
       </c>
       <c r="GH5" s="2">
-        <v>91.608090367261</v>
+        <v>91.60757557609408</v>
       </c>
       <c r="GI5" s="2">
-        <v>91.3443513822827</v>
+        <v>91.35224884165116</v>
       </c>
       <c r="GJ5" s="2">
-        <v>-1.891378694121526</v>
+        <v>-1.92491193822084</v>
       </c>
       <c r="GK5" s="2">
-        <v>4.789825628007571</v>
+        <v>4.799500547109139</v>
       </c>
       <c r="GL5" s="2">
-        <v>3.924230467028092</v>
+        <v>3.928977117192964</v>
       </c>
       <c r="GM5" s="2">
-        <v>3.933981167254206</v>
+        <v>3.943708134004215</v>
       </c>
       <c r="GN5" s="2">
-        <v>7.335198300808786</v>
+        <v>7.330227972449591</v>
       </c>
       <c r="GO5" s="2">
-        <v>2.560389200616851</v>
+        <v>2.569314275385007</v>
       </c>
       <c r="GP5" s="2">
-        <v>9.750874828110954</v>
+        <v>9.760300816613569</v>
       </c>
       <c r="GQ5" s="2">
-        <v>2.130408992168559</v>
+        <v>2.158413717991032</v>
       </c>
       <c r="GR5" s="2">
-        <v>2.849884324386093</v>
+        <v>2.837016282658284</v>
       </c>
       <c r="GS5" s="2">
-        <v>9.119669725453562</v>
+        <v>9.120384594946726</v>
       </c>
       <c r="GT5" s="2">
-        <v>1465.734475575543</v>
+        <v>1461.319736298311</v>
       </c>
       <c r="GU5" s="2">
-        <v>3.60678931436023</v>
+        <v>3.63122194549927</v>
       </c>
       <c r="GV5" s="2">
-        <v>3.608076430668556</v>
+        <v>3.633309682736873</v>
       </c>
       <c r="GW5" s="2">
-        <v>1352.448063727275</v>
+        <v>1349.622318497631</v>
       </c>
       <c r="GX5" s="2">
-        <v>17.08935946896603</v>
+        <v>16.14568936974697</v>
       </c>
       <c r="GY5" s="2">
-        <v>-0.6250598617866446</v>
+        <v>-0.6250593044006202</v>
       </c>
       <c r="GZ5" s="2">
         <v>0.2272727272727273</v>
@@ -4196,49 +3672,49 @@
         <v>0</v>
       </c>
       <c r="HB5" s="2">
-        <v>1.030695517665656</v>
+        <v>1.029575819895404</v>
       </c>
       <c r="HC5" s="2">
-        <v>1245.445112631522</v>
+        <v>1252.482649551554</v>
       </c>
       <c r="HD5" s="2">
-        <v>2283.887845528862</v>
+        <v>2314.012395864129</v>
       </c>
       <c r="HE5" s="2">
         <v>0</v>
       </c>
       <c r="HF5" s="2">
-        <v>846.9696547840269</v>
+        <v>852.2110651613117</v>
       </c>
       <c r="HG5" s="2">
-        <v>1.11946406875849</v>
+        <v>1.118957365420845</v>
       </c>
       <c r="HH5" s="2">
-        <v>79.34137309956571</v>
+        <v>79.77895288171325</v>
       </c>
       <c r="HI5" s="2">
-        <v>89.08993652281094</v>
+        <v>89.43226010045143</v>
       </c>
       <c r="HJ5" s="2">
-        <v>3.082252895411652</v>
+        <v>3.127324864102549</v>
       </c>
       <c r="HK5" s="2">
-        <v>10.29574625042144</v>
+        <v>10.24463530406679</v>
       </c>
       <c r="HL5" s="2">
-        <v>10.14330968989199</v>
+        <v>10.17802963302682</v>
       </c>
       <c r="HM5" s="2">
-        <v>2.226971025084252</v>
+        <v>2.340289502197713</v>
       </c>
       <c r="HN5" s="2">
-        <v>1.391838981557752</v>
+        <v>1.400206783308078</v>
       </c>
       <c r="HO5" s="2">
-        <v>7.330319350453371</v>
+        <v>7.328676090730347</v>
       </c>
       <c r="HP5" s="2">
-        <v>9.499838436366087</v>
+        <v>9.506139520836781</v>
       </c>
       <c r="HQ5" s="2">
         <v>0</v>
@@ -4253,37 +3729,37 @@
         <v>0</v>
       </c>
       <c r="HU5" s="2">
-        <v>42.55602061773435</v>
+        <v>43.31051860996891</v>
       </c>
       <c r="HV5" s="2">
         <v>0.4713688610240334</v>
       </c>
       <c r="HW5" s="2">
-        <v>0.4794035087719299</v>
+        <v>0.4756223893065999</v>
       </c>
       <c r="HX5" s="2">
         <v>0.4543378995433791</v>
       </c>
       <c r="HY5" s="2">
-        <v>0.4686274509803923</v>
+        <v>0.4648148148148149</v>
       </c>
       <c r="HZ5" s="2">
-        <v>279.7996039205533</v>
+        <v>279.3880041666678</v>
       </c>
       <c r="IA5" s="2">
-        <v>8.562664708663283</v>
+        <v>8.563718893078049</v>
       </c>
       <c r="IB5" s="2">
-        <v>4.05780248747921</v>
+        <v>4.068211899473964</v>
       </c>
       <c r="IC5" s="2">
-        <v>8.135929294418013</v>
+        <v>7.917274351794531</v>
       </c>
       <c r="ID5" s="2">
         <v>29.62872505187988</v>
       </c>
       <c r="IE5" s="2">
-        <v>9.819127688830598</v>
+        <v>9.802567590086207</v>
       </c>
       <c r="IF5" s="2">
         <v>0</v>
@@ -4301,28 +3777,28 @@
         <v>0</v>
       </c>
       <c r="IK5" s="2">
-        <v>2.471111846527724</v>
+        <v>2.479882555727137</v>
       </c>
       <c r="IL5" s="2">
-        <v>3.992257287629053</v>
+        <v>4.008808699653184</v>
       </c>
       <c r="IM5" s="2">
-        <v>0.2571608614941324</v>
+        <v>0.2535183641357204</v>
       </c>
       <c r="IN5" s="2">
-        <v>2.611385170503244</v>
+        <v>2.635493579229419</v>
       </c>
       <c r="IO5" s="2">
-        <v>217.9665628932257</v>
+        <v>219.8833119340907</v>
       </c>
       <c r="IP5" s="2">
-        <v>1.376757246699104</v>
+        <v>1.375113012046652</v>
       </c>
       <c r="IQ5" s="2">
-        <v>7.35435655952308</v>
+        <v>7.359938633159794</v>
       </c>
       <c r="IR5" s="2">
-        <v>9.278444387248234</v>
+        <v>9.274767955373479</v>
       </c>
     </row>
   </sheetData>
@@ -4331,507 +3807,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;G</oddHeader>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawingHF r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="19" width="15.7109375" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="5">
-        <v>45717</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1319.851233312598</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1277.365463573899</v>
-      </c>
-      <c r="D4" s="2">
-        <v>555.5347840330222</v>
-      </c>
-      <c r="E4" s="2">
-        <v>8.544852497814363</v>
-      </c>
-      <c r="F4" s="2">
-        <v>127.5639909946694</v>
-      </c>
-      <c r="G4" s="2">
-        <v>560.9665992922477</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2507.113650261539</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.5273675567115854</v>
-      </c>
-      <c r="J4" s="2">
-        <v>104.2177734800965</v>
-      </c>
-      <c r="K4" s="2">
-        <v>196.6018380263553</v>
-      </c>
-      <c r="L4" s="2">
-        <v>3.886327260525569</v>
-      </c>
-      <c r="M4" s="2">
-        <v>3.882120410280882</v>
-      </c>
-      <c r="N4" s="2">
-        <v>9.124538640833684</v>
-      </c>
-      <c r="O4" s="2">
-        <v>10.25044070892182</v>
-      </c>
-      <c r="P4" s="2">
-        <v>1.89226964753697</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>1.155992779280873</v>
-      </c>
-      <c r="R4" s="2">
-        <v>7.660391001929604</v>
-      </c>
-      <c r="S4" s="2">
-        <v>9.172340051414702</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="5">
-        <v>45748</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1320.925141304659</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1288.979545232913</v>
-      </c>
-      <c r="D5" s="2">
-        <v>587.5698348660505</v>
-      </c>
-      <c r="E5" s="2">
-        <v>38.175279731724</v>
-      </c>
-      <c r="F5" s="2">
-        <v>129.2812237122106</v>
-      </c>
-      <c r="G5" s="2">
-        <v>588.0030654638125</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2449.235808673294</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.5984480293666495</v>
-      </c>
-      <c r="J5" s="2">
-        <v>100.5100164461985</v>
-      </c>
-      <c r="K5" s="2">
-        <v>204.4591111008556</v>
-      </c>
-      <c r="L5" s="2">
-        <v>4.049516904225479</v>
-      </c>
-      <c r="M5" s="2">
-        <v>4.04512417111714</v>
-      </c>
-      <c r="N5" s="2">
-        <v>8.861787353458858</v>
-      </c>
-      <c r="O5" s="2">
-        <v>9.753907947205761</v>
-      </c>
-      <c r="P5" s="2">
-        <v>1.102320777936239</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0.9313120685932672</v>
-      </c>
-      <c r="R5" s="2">
-        <v>7.565927862689803</v>
-      </c>
-      <c r="S5" s="2">
-        <v>9.163425479334171</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;G</oddHeader>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawingHF r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="8" width="15.7109375" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="5">
-        <v>45717</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.4666666666666667</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.4333333333333333</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.3125</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.4666666666666666</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2.676277929921118</v>
-      </c>
-      <c r="H4" s="2">
-        <v>4.756905955640744</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="5">
-        <v>45748</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2.471111846527724</v>
-      </c>
-      <c r="H5" s="2">
-        <v>3.992257287629053</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;G</oddHeader>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawingHF r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="5" width="15.7109375" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="5">
-        <v>45717</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>117.4091939759149</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.2744909972812752</v>
-      </c>
-      <c r="E4" s="2">
-        <v>4.171628763109696</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5">
-        <v>45748</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>128.3147064545943</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.2731443782847562</v>
-      </c>
-      <c r="E5" s="2">
-        <v>4.196205452439245</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;G</oddHeader>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawingHF r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="4" width="15.7109375" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5">
-        <v>45717</v>
-      </c>
-      <c r="B4" s="2">
-        <v>261.3778230772805</v>
-      </c>
-      <c r="C4" s="2">
-        <v>8.197852669529452</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3.94591279917999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5">
-        <v>45748</v>
-      </c>
-      <c r="B5" s="2">
-        <v>279.7996039205533</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8.562664708663283</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4.05780248747921</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;G</oddHeader>
+    <oddHeader>&amp;L&amp;G&amp;R&amp;G</oddHeader>
   </headerFooter>
   <drawing r:id="rId1"/>
   <legacyDrawingHF r:id="rId2"/>

</xml_diff>